<commit_message>
Imported excel based product item fixtures
</commit_message>
<xml_diff>
--- a/products/fixtures/XA21.xlsx
+++ b/products/fixtures/XA21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djang\Documents\Soccersystems\products\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA852B45-DC5B-4FF8-B2BB-59281F5CEDF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DE0ABA-701F-4A6E-BB25-B17AC6D4BD23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1080" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products.ProductItem" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="344">
   <si>
     <t>slug</t>
   </si>
@@ -298,36 +298,6 @@
     <t>Naamblok KUDUS</t>
   </si>
   <si>
-    <t>Nr. 0 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 1 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 2 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 3 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 4 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 5 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 6 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 7 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 8 (short)</t>
-  </si>
-  <si>
-    <t>Nr. 9 (short)</t>
-  </si>
-  <si>
     <t>Naamblok IDRISSI</t>
   </si>
   <si>
@@ -349,706 +319,739 @@
     <t>Naamblok ÜNÜVAR</t>
   </si>
   <si>
-    <t>Nr. 0 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 1 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 2 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 3 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 4 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 5 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 6 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 7 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 8 (baby)</t>
-  </si>
-  <si>
-    <t>Nr. 9 (baby)</t>
+    <t>XA21</t>
+  </si>
+  <si>
+    <t>XA21060_</t>
+  </si>
+  <si>
+    <t>XA210600</t>
+  </si>
+  <si>
+    <t>XA21060A</t>
+  </si>
+  <si>
+    <t>XA21060B</t>
+  </si>
+  <si>
+    <t>XA21060C</t>
+  </si>
+  <si>
+    <t>XA21060D</t>
+  </si>
+  <si>
+    <t>XA21060E</t>
+  </si>
+  <si>
+    <t>XA21060F</t>
+  </si>
+  <si>
+    <t>XA21060G</t>
+  </si>
+  <si>
+    <t>XA21060H</t>
+  </si>
+  <si>
+    <t>XA21060I</t>
+  </si>
+  <si>
+    <t>XA21060J</t>
+  </si>
+  <si>
+    <t>XA21060K</t>
+  </si>
+  <si>
+    <t>XA21060L</t>
+  </si>
+  <si>
+    <t>XA21060M</t>
+  </si>
+  <si>
+    <t>XA21060N</t>
+  </si>
+  <si>
+    <t>XA21060O</t>
+  </si>
+  <si>
+    <t>XA21060P</t>
+  </si>
+  <si>
+    <t>XA21060Q</t>
+  </si>
+  <si>
+    <t>XA21060R</t>
+  </si>
+  <si>
+    <t>XA21060S</t>
+  </si>
+  <si>
+    <t>XA21060T</t>
+  </si>
+  <si>
+    <t>XA21060U</t>
+  </si>
+  <si>
+    <t>XA21060V</t>
+  </si>
+  <si>
+    <t>XA21060W</t>
+  </si>
+  <si>
+    <t>XA21060X</t>
+  </si>
+  <si>
+    <t>XA21060Y</t>
+  </si>
+  <si>
+    <t>XA21060Z</t>
+  </si>
+  <si>
+    <t>XA2106AY</t>
+  </si>
+  <si>
+    <t>articles/XA2106AY.svg</t>
+  </si>
+  <si>
+    <t>XA2106AZ</t>
+  </si>
+  <si>
+    <t>articles/XA2106AZ.svg</t>
+  </si>
+  <si>
+    <t>XA2106BD</t>
+  </si>
+  <si>
+    <t>articles/XA2106BD.svg</t>
+  </si>
+  <si>
+    <t>XA2106BY</t>
+  </si>
+  <si>
+    <t>articles/XA2106BY.svg</t>
+  </si>
+  <si>
+    <t>XA2106EP</t>
+  </si>
+  <si>
+    <t>articles/XA2106EP.svg</t>
+  </si>
+  <si>
+    <t>XA2106GH</t>
+  </si>
+  <si>
+    <t>articles/XA2106GH.svg</t>
+  </si>
+  <si>
+    <t>XA2106HE</t>
+  </si>
+  <si>
+    <t>articles/XA2106HE.svg</t>
+  </si>
+  <si>
+    <t>XA2106II</t>
+  </si>
+  <si>
+    <t>articles/XA2106II.svg</t>
+  </si>
+  <si>
+    <t>XA2106JR</t>
+  </si>
+  <si>
+    <t>articles/XA2106JR.svg</t>
+  </si>
+  <si>
+    <t>XA2106KN</t>
+  </si>
+  <si>
+    <t>articles/XA2106KN.svg</t>
+  </si>
+  <si>
+    <t>XA2106KR</t>
+  </si>
+  <si>
+    <t>articles/XA2106KR.svg</t>
+  </si>
+  <si>
+    <t>XA2106KS</t>
+  </si>
+  <si>
+    <t>articles/XA2106KS.svg</t>
+  </si>
+  <si>
+    <t>XA2106LD</t>
+  </si>
+  <si>
+    <t>articles/XA2106LD.svg</t>
+  </si>
+  <si>
+    <t>XA2106MI</t>
+  </si>
+  <si>
+    <t>articles/XA2106MI.svg</t>
+  </si>
+  <si>
+    <t>XA2106MZ</t>
+  </si>
+  <si>
+    <t>articles/XA2106MZ.svg</t>
+  </si>
+  <si>
+    <t>XA2106NS</t>
+  </si>
+  <si>
+    <t>articles/XA2106NS.svg</t>
+  </si>
+  <si>
+    <t>XA2106RH</t>
+  </si>
+  <si>
+    <t>articles/XA2106RH.svg</t>
+  </si>
+  <si>
+    <t>XA2106SS</t>
+  </si>
+  <si>
+    <t>articles/XA2106SS.svg</t>
+  </si>
+  <si>
+    <t>XA2106TC</t>
+  </si>
+  <si>
+    <t>articles/XA2106TC.svg</t>
+  </si>
+  <si>
+    <t>XA2106TE</t>
+  </si>
+  <si>
+    <t>articles/XA2106TE.svg</t>
+  </si>
+  <si>
+    <t>XA2106TO</t>
+  </si>
+  <si>
+    <t>articles/XA2106TO.svg</t>
+  </si>
+  <si>
+    <t>XA2106TR</t>
+  </si>
+  <si>
+    <t>articles/XA2106TR.svg</t>
+  </si>
+  <si>
+    <t>XA2106UR</t>
+  </si>
+  <si>
+    <t>articles/XA2106UR.svg</t>
+  </si>
+  <si>
+    <t>XA210900</t>
+  </si>
+  <si>
+    <t>articles/XA210900.svg</t>
+  </si>
+  <si>
+    <t>XA210901</t>
+  </si>
+  <si>
+    <t>articles/XA210901.svg</t>
+  </si>
+  <si>
+    <t>XA210902</t>
+  </si>
+  <si>
+    <t>articles/XA210902.svg</t>
+  </si>
+  <si>
+    <t>XA210903</t>
+  </si>
+  <si>
+    <t>articles/XA210903.svg</t>
+  </si>
+  <si>
+    <t>XA210904</t>
+  </si>
+  <si>
+    <t>articles/XA210904.svg</t>
+  </si>
+  <si>
+    <t>XA210905</t>
+  </si>
+  <si>
+    <t>articles/XA210905.svg</t>
+  </si>
+  <si>
+    <t>XA210906</t>
+  </si>
+  <si>
+    <t>articles/XA210906.svg</t>
+  </si>
+  <si>
+    <t>XA210907</t>
+  </si>
+  <si>
+    <t>articles/XA210907.svg</t>
+  </si>
+  <si>
+    <t>XA210908</t>
+  </si>
+  <si>
+    <t>articles/XA210908.svg</t>
+  </si>
+  <si>
+    <t>XA210909</t>
+  </si>
+  <si>
+    <t>articles/XA210909.svg</t>
+  </si>
+  <si>
+    <t>XA211000</t>
+  </si>
+  <si>
+    <t>articles/XA211000.svg</t>
+  </si>
+  <si>
+    <t>XA211001</t>
+  </si>
+  <si>
+    <t>articles/XA211001.svg</t>
+  </si>
+  <si>
+    <t>XA211002</t>
+  </si>
+  <si>
+    <t>articles/XA211002.svg</t>
+  </si>
+  <si>
+    <t>XA211003</t>
+  </si>
+  <si>
+    <t>articles/XA211003.svg</t>
+  </si>
+  <si>
+    <t>XA211004</t>
+  </si>
+  <si>
+    <t>articles/XA211004.svg</t>
+  </si>
+  <si>
+    <t>XA211005</t>
+  </si>
+  <si>
+    <t>articles/XA211005.svg</t>
+  </si>
+  <si>
+    <t>XA211006</t>
+  </si>
+  <si>
+    <t>articles/XA211006.svg</t>
+  </si>
+  <si>
+    <t>XA211007</t>
+  </si>
+  <si>
+    <t>articles/XA211007.svg</t>
+  </si>
+  <si>
+    <t>XA211008</t>
+  </si>
+  <si>
+    <t>articles/XA211008.svg</t>
+  </si>
+  <si>
+    <t>XA211009</t>
+  </si>
+  <si>
+    <t>articles/XA211009.svg</t>
+  </si>
+  <si>
+    <t>XA211600</t>
+  </si>
+  <si>
+    <t>articles/XA211600.svg</t>
+  </si>
+  <si>
+    <t>XA211601</t>
+  </si>
+  <si>
+    <t>articles/XA211601.svg</t>
+  </si>
+  <si>
+    <t>XA211602</t>
+  </si>
+  <si>
+    <t>articles/XA211602.svg</t>
+  </si>
+  <si>
+    <t>XA211603</t>
+  </si>
+  <si>
+    <t>articles/XA211603.svg</t>
+  </si>
+  <si>
+    <t>XA211604</t>
+  </si>
+  <si>
+    <t>articles/XA211604.svg</t>
+  </si>
+  <si>
+    <t>XA211605</t>
+  </si>
+  <si>
+    <t>articles/XA211605.svg</t>
+  </si>
+  <si>
+    <t>XA211606</t>
+  </si>
+  <si>
+    <t>articles/XA211606.svg</t>
+  </si>
+  <si>
+    <t>XA211607</t>
+  </si>
+  <si>
+    <t>articles/XA211607.svg</t>
+  </si>
+  <si>
+    <t>XA211608</t>
+  </si>
+  <si>
+    <t>articles/XA211608.svg</t>
+  </si>
+  <si>
+    <t>XA211609</t>
+  </si>
+  <si>
+    <t>articles/XA211609.svg</t>
+  </si>
+  <si>
+    <t>XA212500</t>
+  </si>
+  <si>
+    <t>articles/XA212500.svg</t>
+  </si>
+  <si>
+    <t>XA212501</t>
+  </si>
+  <si>
+    <t>articles/XA212501.svg</t>
+  </si>
+  <si>
+    <t>XA212502</t>
+  </si>
+  <si>
+    <t>articles/XA212502.svg</t>
+  </si>
+  <si>
+    <t>XA212503</t>
+  </si>
+  <si>
+    <t>articles/XA212503.svg</t>
+  </si>
+  <si>
+    <t>XA212504</t>
+  </si>
+  <si>
+    <t>articles/XA212504.svg</t>
+  </si>
+  <si>
+    <t>XA212505</t>
+  </si>
+  <si>
+    <t>articles/XA212505.svg</t>
+  </si>
+  <si>
+    <t>XA212506</t>
+  </si>
+  <si>
+    <t>articles/XA212506.svg</t>
+  </si>
+  <si>
+    <t>XA212507</t>
+  </si>
+  <si>
+    <t>articles/XA212507.svg</t>
+  </si>
+  <si>
+    <t>XA212508</t>
+  </si>
+  <si>
+    <t>articles/XA212508.svg</t>
+  </si>
+  <si>
+    <t>XA212509</t>
+  </si>
+  <si>
+    <t>articles/XA212509.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060_.svg</t>
+  </si>
+  <si>
+    <t>articles/XA210600.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060A.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060B.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060C.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060D.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060E.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060F.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060G.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060H.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060I.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060J.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060K.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060L.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060M.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060N.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060O.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060P.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060Q.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060R.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060S.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060T.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060U.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060V.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060W.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060X.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060Y.svg</t>
+  </si>
+  <si>
+    <t>articles/XA21060Z.svg</t>
   </si>
   <si>
     <t>XA21040_</t>
   </si>
   <si>
-    <t>XA21</t>
-  </si>
-  <si>
-    <t>articles/XA21040_.svg</t>
-  </si>
-  <si>
     <t>XA210400</t>
   </si>
   <si>
-    <t>articles/XA210400.svg</t>
-  </si>
-  <si>
     <t>XA21040A</t>
   </si>
   <si>
-    <t>articles/XA21040A.svg</t>
-  </si>
-  <si>
     <t>XA21040B</t>
   </si>
   <si>
-    <t>articles/XA21040B.svg</t>
-  </si>
-  <si>
     <t>XA21040C</t>
   </si>
   <si>
-    <t>articles/XA21040C.svg</t>
-  </si>
-  <si>
     <t>XA21040D</t>
   </si>
   <si>
-    <t>articles/XA21040D.svg</t>
-  </si>
-  <si>
     <t>XA21040E</t>
   </si>
   <si>
-    <t>articles/XA21040E.svg</t>
-  </si>
-  <si>
     <t>XA21040F</t>
   </si>
   <si>
-    <t>articles/XA21040F.svg</t>
-  </si>
-  <si>
     <t>XA21040G</t>
   </si>
   <si>
-    <t>articles/XA21040G.svg</t>
-  </si>
-  <si>
     <t>XA21040H</t>
   </si>
   <si>
-    <t>articles/XA21040H.svg</t>
-  </si>
-  <si>
     <t>XA21040I</t>
   </si>
   <si>
-    <t>articles/XA21040I.svg</t>
-  </si>
-  <si>
     <t>XA21040J</t>
   </si>
   <si>
-    <t>articles/XA21040J.svg</t>
-  </si>
-  <si>
     <t>XA21040K</t>
   </si>
   <si>
-    <t>articles/XA21040K.svg</t>
-  </si>
-  <si>
     <t>XA21040L</t>
   </si>
   <si>
-    <t>articles/XA21040L.svg</t>
-  </si>
-  <si>
     <t>XA21040M</t>
   </si>
   <si>
-    <t>articles/XA21040M.svg</t>
-  </si>
-  <si>
     <t>XA21040N</t>
   </si>
   <si>
-    <t>articles/XA21040N.svg</t>
-  </si>
-  <si>
     <t>XA21040O</t>
   </si>
   <si>
-    <t>articles/XA21040O.svg</t>
-  </si>
-  <si>
     <t>XA21040P</t>
   </si>
   <si>
-    <t>articles/XA21040P.svg</t>
-  </si>
-  <si>
     <t>XA21040Q</t>
   </si>
   <si>
-    <t>articles/XA21040Q.svg</t>
-  </si>
-  <si>
     <t>XA21040R</t>
   </si>
   <si>
-    <t>articles/XA21040R.svg</t>
-  </si>
-  <si>
     <t>XA21040S</t>
   </si>
   <si>
-    <t>articles/XA21040S.svg</t>
-  </si>
-  <si>
     <t>XA21040T</t>
   </si>
   <si>
-    <t>articles/XA21040T.svg</t>
-  </si>
-  <si>
     <t>XA21040U</t>
   </si>
   <si>
-    <t>articles/XA21040U.svg</t>
-  </si>
-  <si>
     <t>XA21040V</t>
   </si>
   <si>
-    <t>articles/XA21040V.svg</t>
-  </si>
-  <si>
     <t>XA21040W</t>
   </si>
   <si>
-    <t>articles/XA21040W.svg</t>
-  </si>
-  <si>
     <t>XA21040X</t>
   </si>
   <si>
-    <t>articles/XA21040X.svg</t>
-  </si>
-  <si>
     <t>XA21040Y</t>
   </si>
   <si>
-    <t>articles/XA21040Y.svg</t>
-  </si>
-  <si>
     <t>XA21040Z</t>
   </si>
   <si>
-    <t>articles/XA21040Z.svg</t>
-  </si>
-  <si>
-    <t>XA21060_</t>
-  </si>
-  <si>
-    <t>XA210600</t>
-  </si>
-  <si>
-    <t>XA21060A</t>
-  </si>
-  <si>
-    <t>XA21060B</t>
-  </si>
-  <si>
-    <t>XA21060C</t>
-  </si>
-  <si>
-    <t>XA21060D</t>
-  </si>
-  <si>
-    <t>XA21060E</t>
-  </si>
-  <si>
-    <t>XA21060F</t>
-  </si>
-  <si>
-    <t>XA21060G</t>
-  </si>
-  <si>
-    <t>XA21060H</t>
-  </si>
-  <si>
-    <t>XA21060I</t>
-  </si>
-  <si>
-    <t>XA21060J</t>
-  </si>
-  <si>
-    <t>XA21060K</t>
-  </si>
-  <si>
-    <t>XA21060L</t>
-  </si>
-  <si>
-    <t>XA21060M</t>
-  </si>
-  <si>
-    <t>XA21060N</t>
-  </si>
-  <si>
-    <t>XA21060O</t>
-  </si>
-  <si>
-    <t>XA21060P</t>
-  </si>
-  <si>
-    <t>XA21060Q</t>
-  </si>
-  <si>
-    <t>XA21060R</t>
-  </si>
-  <si>
-    <t>XA21060S</t>
-  </si>
-  <si>
-    <t>XA21060T</t>
-  </si>
-  <si>
-    <t>XA21060U</t>
-  </si>
-  <si>
-    <t>XA21060V</t>
-  </si>
-  <si>
-    <t>XA21060W</t>
-  </si>
-  <si>
-    <t>XA21060X</t>
-  </si>
-  <si>
-    <t>XA21060Y</t>
-  </si>
-  <si>
-    <t>XA21060Z</t>
-  </si>
-  <si>
-    <t>XA2106AY</t>
-  </si>
-  <si>
-    <t>articles/XA2106AY.svg</t>
-  </si>
-  <si>
-    <t>XA2106AZ</t>
-  </si>
-  <si>
-    <t>articles/XA2106AZ.svg</t>
-  </si>
-  <si>
-    <t>XA2106BD</t>
-  </si>
-  <si>
-    <t>articles/XA2106BD.svg</t>
-  </si>
-  <si>
-    <t>XA2106BY</t>
-  </si>
-  <si>
-    <t>articles/XA2106BY.svg</t>
-  </si>
-  <si>
-    <t>XA2106EP</t>
-  </si>
-  <si>
-    <t>articles/XA2106EP.svg</t>
-  </si>
-  <si>
-    <t>XA2106GH</t>
-  </si>
-  <si>
-    <t>articles/XA2106GH.svg</t>
-  </si>
-  <si>
-    <t>XA2106HE</t>
-  </si>
-  <si>
-    <t>articles/XA2106HE.svg</t>
-  </si>
-  <si>
-    <t>XA2106II</t>
-  </si>
-  <si>
-    <t>articles/XA2106II.svg</t>
-  </si>
-  <si>
-    <t>XA2106JR</t>
-  </si>
-  <si>
-    <t>articles/XA2106JR.svg</t>
-  </si>
-  <si>
-    <t>XA2106KN</t>
-  </si>
-  <si>
-    <t>articles/XA2106KN.svg</t>
-  </si>
-  <si>
-    <t>XA2106KR</t>
-  </si>
-  <si>
-    <t>articles/XA2106KR.svg</t>
-  </si>
-  <si>
-    <t>XA2106KS</t>
-  </si>
-  <si>
-    <t>articles/XA2106KS.svg</t>
-  </si>
-  <si>
-    <t>XA2106LD</t>
-  </si>
-  <si>
-    <t>articles/XA2106LD.svg</t>
-  </si>
-  <si>
-    <t>XA2106MI</t>
-  </si>
-  <si>
-    <t>articles/XA2106MI.svg</t>
-  </si>
-  <si>
-    <t>XA2106MZ</t>
-  </si>
-  <si>
-    <t>articles/XA2106MZ.svg</t>
-  </si>
-  <si>
-    <t>XA2106NS</t>
-  </si>
-  <si>
-    <t>articles/XA2106NS.svg</t>
-  </si>
-  <si>
-    <t>XA2106RH</t>
-  </si>
-  <si>
-    <t>articles/XA2106RH.svg</t>
-  </si>
-  <si>
-    <t>XA2106SS</t>
-  </si>
-  <si>
-    <t>articles/XA2106SS.svg</t>
-  </si>
-  <si>
-    <t>XA2106TC</t>
-  </si>
-  <si>
-    <t>articles/XA2106TC.svg</t>
-  </si>
-  <si>
-    <t>XA2106TE</t>
-  </si>
-  <si>
-    <t>articles/XA2106TE.svg</t>
-  </si>
-  <si>
-    <t>XA2106TO</t>
-  </si>
-  <si>
-    <t>articles/XA2106TO.svg</t>
-  </si>
-  <si>
-    <t>XA2106TR</t>
-  </si>
-  <si>
-    <t>articles/XA2106TR.svg</t>
-  </si>
-  <si>
-    <t>XA2106UR</t>
-  </si>
-  <si>
-    <t>articles/XA2106UR.svg</t>
-  </si>
-  <si>
-    <t>XA210900</t>
-  </si>
-  <si>
-    <t>articles/XA210900.svg</t>
-  </si>
-  <si>
-    <t>XA210901</t>
-  </si>
-  <si>
-    <t>articles/XA210901.svg</t>
-  </si>
-  <si>
-    <t>XA210902</t>
-  </si>
-  <si>
-    <t>articles/XA210902.svg</t>
-  </si>
-  <si>
-    <t>XA210903</t>
-  </si>
-  <si>
-    <t>articles/XA210903.svg</t>
-  </si>
-  <si>
-    <t>XA210904</t>
-  </si>
-  <si>
-    <t>articles/XA210904.svg</t>
-  </si>
-  <si>
-    <t>XA210905</t>
-  </si>
-  <si>
-    <t>articles/XA210905.svg</t>
-  </si>
-  <si>
-    <t>XA210906</t>
-  </si>
-  <si>
-    <t>articles/XA210906.svg</t>
-  </si>
-  <si>
-    <t>XA210907</t>
-  </si>
-  <si>
-    <t>articles/XA210907.svg</t>
-  </si>
-  <si>
-    <t>XA210908</t>
-  </si>
-  <si>
-    <t>articles/XA210908.svg</t>
-  </si>
-  <si>
-    <t>XA210909</t>
-  </si>
-  <si>
-    <t>articles/XA210909.svg</t>
-  </si>
-  <si>
-    <t>XA211000</t>
-  </si>
-  <si>
-    <t>articles/XA211000.svg</t>
-  </si>
-  <si>
-    <t>XA211001</t>
-  </si>
-  <si>
-    <t>articles/XA211001.svg</t>
-  </si>
-  <si>
-    <t>XA211002</t>
-  </si>
-  <si>
-    <t>articles/XA211002.svg</t>
-  </si>
-  <si>
-    <t>XA211003</t>
-  </si>
-  <si>
-    <t>articles/XA211003.svg</t>
-  </si>
-  <si>
-    <t>XA211004</t>
-  </si>
-  <si>
-    <t>articles/XA211004.svg</t>
-  </si>
-  <si>
-    <t>XA211005</t>
-  </si>
-  <si>
-    <t>articles/XA211005.svg</t>
-  </si>
-  <si>
-    <t>XA211006</t>
-  </si>
-  <si>
-    <t>articles/XA211006.svg</t>
-  </si>
-  <si>
-    <t>XA211007</t>
-  </si>
-  <si>
-    <t>articles/XA211007.svg</t>
-  </si>
-  <si>
-    <t>XA211008</t>
-  </si>
-  <si>
-    <t>articles/XA211008.svg</t>
-  </si>
-  <si>
-    <t>XA211009</t>
-  </si>
-  <si>
-    <t>articles/XA211009.svg</t>
-  </si>
-  <si>
-    <t>XA211600</t>
-  </si>
-  <si>
-    <t>articles/XA211600.svg</t>
-  </si>
-  <si>
-    <t>XA211601</t>
-  </si>
-  <si>
-    <t>articles/XA211601.svg</t>
-  </si>
-  <si>
-    <t>XA211602</t>
-  </si>
-  <si>
-    <t>articles/XA211602.svg</t>
-  </si>
-  <si>
-    <t>XA211603</t>
-  </si>
-  <si>
-    <t>articles/XA211603.svg</t>
-  </si>
-  <si>
-    <t>XA211604</t>
-  </si>
-  <si>
-    <t>articles/XA211604.svg</t>
-  </si>
-  <si>
-    <t>XA211605</t>
-  </si>
-  <si>
-    <t>articles/XA211605.svg</t>
-  </si>
-  <si>
-    <t>XA211606</t>
-  </si>
-  <si>
-    <t>articles/XA211606.svg</t>
-  </si>
-  <si>
-    <t>XA211607</t>
-  </si>
-  <si>
-    <t>articles/XA211607.svg</t>
-  </si>
-  <si>
-    <t>XA211608</t>
-  </si>
-  <si>
-    <t>articles/XA211608.svg</t>
-  </si>
-  <si>
-    <t>XA211609</t>
-  </si>
-  <si>
-    <t>articles/XA211609.svg</t>
-  </si>
-  <si>
-    <t>XA212500</t>
-  </si>
-  <si>
-    <t>articles/XA212500.svg</t>
-  </si>
-  <si>
-    <t>XA212501</t>
-  </si>
-  <si>
-    <t>articles/XA212501.svg</t>
-  </si>
-  <si>
-    <t>XA212502</t>
-  </si>
-  <si>
-    <t>articles/XA212502.svg</t>
-  </si>
-  <si>
-    <t>XA212503</t>
-  </si>
-  <si>
-    <t>articles/XA212503.svg</t>
-  </si>
-  <si>
-    <t>XA212504</t>
-  </si>
-  <si>
-    <t>articles/XA212504.svg</t>
-  </si>
-  <si>
-    <t>XA212505</t>
-  </si>
-  <si>
-    <t>articles/XA212505.svg</t>
-  </si>
-  <si>
-    <t>XA212506</t>
-  </si>
-  <si>
-    <t>articles/XA212506.svg</t>
-  </si>
-  <si>
-    <t>XA212507</t>
-  </si>
-  <si>
-    <t>articles/XA212507.svg</t>
-  </si>
-  <si>
-    <t>XA212508</t>
-  </si>
-  <si>
-    <t>articles/XA212508.svg</t>
-  </si>
-  <si>
-    <t>XA212509</t>
-  </si>
-  <si>
-    <t>articles/XA212509.svg</t>
-  </si>
-  <si>
-    <t>00215169</t>
-  </si>
-  <si>
-    <t>00912140</t>
-  </si>
-  <si>
-    <t>02233360</t>
-  </si>
-  <si>
-    <t>04516636</t>
-  </si>
-  <si>
-    <t>07101665</t>
-  </si>
-  <si>
-    <t>01575552</t>
-  </si>
-  <si>
-    <t>02077619</t>
-  </si>
-  <si>
-    <t>05139991</t>
-  </si>
-  <si>
-    <t>00708985</t>
-  </si>
-  <si>
-    <t>08226602</t>
-  </si>
-  <si>
-    <t>03748807</t>
-  </si>
-  <si>
-    <t>02698366</t>
-  </si>
-  <si>
-    <t>07366639</t>
+    <t>01306435</t>
+  </si>
+  <si>
+    <t>03077119</t>
+  </si>
+  <si>
+    <t>05204901</t>
+  </si>
+  <si>
+    <t>06723159</t>
+  </si>
+  <si>
+    <t>03005203</t>
+  </si>
+  <si>
+    <t>04828830</t>
+  </si>
+  <si>
+    <t>06228958</t>
+  </si>
+  <si>
+    <t>07861089</t>
+  </si>
+  <si>
+    <t>06212746</t>
+  </si>
+  <si>
+    <t>08453540</t>
+  </si>
+  <si>
+    <t>00292763</t>
+  </si>
+  <si>
+    <t>05455658</t>
+  </si>
+  <si>
+    <t>07956905</t>
+  </si>
+  <si>
+    <t>02213260</t>
+  </si>
+  <si>
+    <t>Nr. 0 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 1 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 2 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 0 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 1 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 2 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 3 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 4 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 5 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 6 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 7 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 8 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 9 (short 1 - baby)</t>
+  </si>
+  <si>
+    <t>Nr. 3 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 4 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 5 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 6 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 7 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 8 (short 2)</t>
+  </si>
+  <si>
+    <t>Nr. 9 (short 2)</t>
   </si>
 </sst>
 </file>
@@ -1426,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,19 +1481,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>282</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="8">
-        <v>66294575</v>
+        <v>83018943</v>
       </c>
       <c r="E2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F2" s="2">
         <v>4</v>
@@ -1502,22 +1505,22 @@
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="8">
-        <v>23463452</v>
+      <c r="D3" s="8" t="s">
+        <v>310</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -1532,22 +1535,22 @@
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>123</v>
+        <v>255</v>
       </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" s="8">
-        <v>41003681</v>
+        <v>92789740</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1562,21 +1565,21 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>125</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="8">
-        <v>25497166</v>
+        <v>50681036</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -1591,21 +1594,21 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>127</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="8">
-        <v>63547363</v>
+        <v>96407959</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1620,21 +1623,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>287</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="8">
-        <v>55181312</v>
+        <v>13808563</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1649,21 +1652,21 @@
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>131</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>288</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" s="8">
-        <v>63057604</v>
+        <v>22383167</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -1678,21 +1681,21 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>133</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>289</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>330</v>
+      <c r="D9" s="8">
+        <v>84599867</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -1707,21 +1710,21 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>135</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>290</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="8">
-        <v>69063528</v>
+        <v>92443765</v>
       </c>
       <c r="E10" t="s">
         <v>17</v>
@@ -1736,21 +1739,21 @@
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>291</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="8">
-        <v>68940053</v>
+        <v>72579256</v>
       </c>
       <c r="E11" t="s">
         <v>18</v>
@@ -1765,21 +1768,21 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>292</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>331</v>
+      <c r="D12" s="8">
+        <v>18108960</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -1794,21 +1797,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>293</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" s="8">
-        <v>87052367</v>
+        <v>59366270</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
@@ -1823,21 +1826,21 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>143</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>294</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="8">
-        <v>58410124</v>
+        <v>21121821</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
@@ -1852,21 +1855,21 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>145</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15" s="8">
-        <v>49153691</v>
+        <v>38767764</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -1881,21 +1884,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>147</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" s="8">
-        <v>28437697</v>
+        <v>21600396</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
@@ -1910,21 +1913,21 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>149</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-      <c r="D17" s="8">
-        <v>68493865</v>
+      <c r="D17" s="8" t="s">
+        <v>311</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
@@ -1939,21 +1942,21 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" s="8">
-        <v>72062139</v>
+        <v>29240238</v>
       </c>
       <c r="E18" t="s">
         <v>25</v>
@@ -1968,21 +1971,21 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>153</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>299</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" s="8">
-        <v>74486054</v>
+        <v>19974648</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
@@ -1997,21 +2000,21 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>155</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C20">
         <v>2</v>
       </c>
       <c r="D20" s="8">
-        <v>94863215</v>
+        <v>54567076</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
@@ -2026,21 +2029,21 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>157</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>158</v>
+        <v>301</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="8">
-        <v>92216569</v>
+      <c r="D21" s="8" t="s">
+        <v>312</v>
       </c>
       <c r="E21" t="s">
         <v>28</v>
@@ -2055,21 +2058,21 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>302</v>
       </c>
       <c r="B22" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>332</v>
+      <c r="D22" s="8">
+        <v>21366472</v>
       </c>
       <c r="E22" t="s">
         <v>29</v>
@@ -2084,21 +2087,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>161</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>303</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23" s="8">
-        <v>47581048</v>
+        <v>89350499</v>
       </c>
       <c r="E23" t="s">
         <v>30</v>
@@ -2113,21 +2116,21 @@
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>163</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>164</v>
+        <v>304</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24" s="8">
-        <v>33537183</v>
+        <v>12532079</v>
       </c>
       <c r="E24" t="s">
         <v>31</v>
@@ -2142,21 +2145,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>165</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>305</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>333</v>
+      <c r="D25" s="8">
+        <v>48362297</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -2171,21 +2174,21 @@
         <v>0</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" s="8">
-        <v>72152627</v>
+        <v>80130123</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -2200,21 +2203,21 @@
         <v>0</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>169</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>307</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C27">
         <v>2</v>
       </c>
       <c r="D27" s="8">
-        <v>81189414</v>
+        <v>85134386</v>
       </c>
       <c r="E27" t="s">
         <v>34</v>
@@ -2229,21 +2232,21 @@
         <v>0</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>172</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
       <c r="D28" s="8">
-        <v>80672735</v>
+        <v>90905649</v>
       </c>
       <c r="E28" t="s">
         <v>35</v>
@@ -2258,21 +2261,21 @@
         <v>0</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>173</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>309</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" s="8">
-        <v>33936283</v>
+        <v>20630060</v>
       </c>
       <c r="E29" t="s">
         <v>36</v>
@@ -2287,21 +2290,21 @@
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>175</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
       <c r="D30" s="8">
-        <v>37416376</v>
+        <v>85604440</v>
       </c>
       <c r="E30" t="s">
         <v>37</v>
@@ -2316,21 +2319,21 @@
         <v>0</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>121</v>
+        <v>254</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C31">
         <v>2</v>
       </c>
       <c r="D31" s="8">
-        <v>57591490</v>
+        <v>35875272</v>
       </c>
       <c r="E31" t="s">
         <v>38</v>
@@ -2345,21 +2348,21 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>123</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>178</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32" s="8">
-        <v>72603300</v>
+        <v>46846534</v>
       </c>
       <c r="E32" t="s">
         <v>39</v>
@@ -2374,21 +2377,21 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>125</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" s="8">
-        <v>34066194</v>
+        <v>55119603</v>
       </c>
       <c r="E33" t="s">
         <v>40</v>
@@ -2403,21 +2406,21 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>127</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>180</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" s="8">
-        <v>27728833</v>
+        <v>36188598</v>
       </c>
       <c r="E34" t="s">
         <v>41</v>
@@ -2432,21 +2435,21 @@
         <v>0</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35" s="8">
-        <v>48593880</v>
+        <v>42894729</v>
       </c>
       <c r="E35" t="s">
         <v>42</v>
@@ -2461,21 +2464,21 @@
         <v>0</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>131</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36" s="8">
-        <v>46497022</v>
+        <v>70242057</v>
       </c>
       <c r="E36" t="s">
         <v>43</v>
@@ -2490,21 +2493,21 @@
         <v>0</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>133</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" s="8">
-        <v>98231335</v>
+        <v>64804285</v>
       </c>
       <c r="E37" t="s">
         <v>44</v>
@@ -2519,21 +2522,21 @@
         <v>0</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>135</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>184</v>
+        <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C38">
         <v>2</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>334</v>
+      <c r="D38" s="8">
+        <v>32863248</v>
       </c>
       <c r="E38" t="s">
         <v>45</v>
@@ -2548,21 +2551,21 @@
         <v>0</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>185</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" s="8">
-        <v>49869441</v>
+        <v>99024920</v>
       </c>
       <c r="E39" t="s">
         <v>46</v>
@@ -2577,21 +2580,21 @@
         <v>0</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>139</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40" s="8">
-        <v>69849104</v>
+        <v>34283835</v>
       </c>
       <c r="E40" t="s">
         <v>47</v>
@@ -2606,21 +2609,21 @@
         <v>0</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>141</v>
+        <v>264</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C41">
         <v>2</v>
       </c>
       <c r="D41" s="8">
-        <v>21351350</v>
+        <v>94832032</v>
       </c>
       <c r="E41" t="s">
         <v>48</v>
@@ -2635,21 +2638,21 @@
         <v>0</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>143</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C42">
         <v>2</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>335</v>
+      <c r="D42" s="8">
+        <v>58032721</v>
       </c>
       <c r="E42" t="s">
         <v>49</v>
@@ -2664,21 +2667,21 @@
         <v>0</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>145</v>
+        <v>266</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>189</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43" s="8">
-        <v>60478683</v>
+        <v>47441858</v>
       </c>
       <c r="E43" t="s">
         <v>50</v>
@@ -2693,21 +2696,21 @@
         <v>0</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>147</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>190</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44" s="8">
-        <v>89058304</v>
+        <v>52331603</v>
       </c>
       <c r="E44" t="s">
         <v>51</v>
@@ -2722,21 +2725,21 @@
         <v>0</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>149</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>191</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45" s="8">
-        <v>81294390</v>
+        <v>53270683</v>
       </c>
       <c r="E45" t="s">
         <v>52</v>
@@ -2751,21 +2754,21 @@
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>151</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>192</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" s="8">
-        <v>39777494</v>
+        <v>85452317</v>
       </c>
       <c r="E46" t="s">
         <v>53</v>
@@ -2780,21 +2783,21 @@
         <v>0</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>153</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47" s="8">
-        <v>80320760</v>
+        <v>87667265</v>
       </c>
       <c r="E47" t="s">
         <v>54</v>
@@ -2809,21 +2812,21 @@
         <v>0</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>155</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C48">
         <v>2</v>
       </c>
-      <c r="D48" s="8">
-        <v>42717400</v>
+      <c r="D48" s="8" t="s">
+        <v>313</v>
       </c>
       <c r="E48" t="s">
         <v>55</v>
@@ -2838,21 +2841,21 @@
         <v>0</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>157</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C49">
         <v>2</v>
       </c>
       <c r="D49" s="8">
-        <v>20655231</v>
+        <v>64340495</v>
       </c>
       <c r="E49" t="s">
         <v>56</v>
@@ -2867,21 +2870,21 @@
         <v>0</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C50">
         <v>2</v>
       </c>
       <c r="D50" s="8">
-        <v>24253278</v>
+        <v>37215080</v>
       </c>
       <c r="E50" t="s">
         <v>57</v>
@@ -2896,21 +2899,21 @@
         <v>0</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>161</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>197</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
-      <c r="D51" s="8">
-        <v>60661624</v>
+      <c r="D51" s="8" t="s">
+        <v>314</v>
       </c>
       <c r="E51" t="s">
         <v>58</v>
@@ -2925,21 +2928,21 @@
         <v>0</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>163</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
       <c r="D52" s="8">
-        <v>26292839</v>
+        <v>43724266</v>
       </c>
       <c r="E52" t="s">
         <v>59</v>
@@ -2954,21 +2957,21 @@
         <v>0</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>165</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>199</v>
+        <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
       <c r="D53" s="8">
-        <v>48809033</v>
+        <v>96116282</v>
       </c>
       <c r="E53" t="s">
         <v>60</v>
@@ -2983,21 +2986,21 @@
         <v>0</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>167</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>200</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C54">
         <v>2</v>
       </c>
       <c r="D54" s="8">
-        <v>95680325</v>
+        <v>34708583</v>
       </c>
       <c r="E54" t="s">
         <v>61</v>
@@ -3012,21 +3015,21 @@
         <v>0</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>169</v>
+        <v>278</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C55">
         <v>2</v>
       </c>
       <c r="D55" s="8">
-        <v>70166165</v>
+        <v>26422898</v>
       </c>
       <c r="E55" t="s">
         <v>62</v>
@@ -3041,21 +3044,21 @@
         <v>0</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>171</v>
+        <v>279</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>202</v>
+        <v>126</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
       <c r="D56" s="8">
-        <v>45542867</v>
+        <v>34455382</v>
       </c>
       <c r="E56" t="s">
         <v>63</v>
@@ -3070,21 +3073,21 @@
         <v>0</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>173</v>
+        <v>280</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>203</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C57">
         <v>2</v>
       </c>
       <c r="D57" s="8">
-        <v>99701577</v>
+        <v>93448342</v>
       </c>
       <c r="E57" t="s">
         <v>64</v>
@@ -3099,21 +3102,21 @@
         <v>0</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>175</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>204</v>
+        <v>128</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" s="8">
-        <v>69675381</v>
+        <v>75179725</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>65</v>
@@ -3128,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>205</v>
+        <v>129</v>
       </c>
       <c r="J58">
         <v>2</v>
@@ -3136,19 +3139,19 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>206</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" s="8">
-        <v>97310114</v>
+        <v>72207496</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="F59">
         <v>6</v>
@@ -3160,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>207</v>
+        <v>131</v>
       </c>
       <c r="J59">
         <v>2</v>
@@ -3168,16 +3171,16 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>208</v>
+        <v>132</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" s="8">
-        <v>81765974</v>
+        <v>37179586</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>66</v>
@@ -3192,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>209</v>
+        <v>133</v>
       </c>
       <c r="J60">
         <v>2</v>
@@ -3200,16 +3203,16 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>210</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" s="8">
-        <v>76357752</v>
+        <v>84497554</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>67</v>
@@ -3224,7 +3227,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>211</v>
+        <v>135</v>
       </c>
       <c r="J61">
         <v>2</v>
@@ -3232,16 +3235,16 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>212</v>
+        <v>136</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="D62" s="8" t="s">
-        <v>336</v>
+      <c r="D62" s="8">
+        <v>51594934</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>68</v>
@@ -3256,7 +3259,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="J62">
         <v>2</v>
@@ -3264,16 +3267,16 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>214</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" s="8">
-        <v>44364699</v>
+        <v>49846331</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>69</v>
@@ -3288,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>215</v>
+        <v>139</v>
       </c>
       <c r="J63">
         <v>2</v>
@@ -3296,16 +3299,16 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>216</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" s="8">
-        <v>76497632</v>
+        <v>17543268</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>70</v>
@@ -3320,7 +3323,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>217</v>
+        <v>141</v>
       </c>
       <c r="J64">
         <v>2</v>
@@ -3328,19 +3331,19 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>218</v>
+        <v>142</v>
       </c>
       <c r="B65" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" s="8">
-        <v>46868161</v>
+        <v>52149738</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="F65">
         <v>6</v>
@@ -3352,7 +3355,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>219</v>
+        <v>143</v>
       </c>
       <c r="J65">
         <v>2</v>
@@ -3360,16 +3363,16 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>220</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" s="8">
-        <v>18559613</v>
+        <v>22563889</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>71</v>
@@ -3384,7 +3387,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>221</v>
+        <v>145</v>
       </c>
       <c r="J66">
         <v>2</v>
@@ -3392,16 +3395,16 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>222</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" s="8">
-        <v>41674808</v>
+        <v>56893477</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>72</v>
@@ -3416,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>223</v>
+        <v>147</v>
       </c>
       <c r="J67">
         <v>2</v>
@@ -3424,16 +3427,16 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>224</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
-      <c r="D68" s="8" t="s">
-        <v>337</v>
+      <c r="D68" s="8">
+        <v>70743624</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>73</v>
@@ -3448,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>225</v>
+        <v>149</v>
       </c>
       <c r="J68">
         <v>2</v>
@@ -3456,16 +3459,16 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>226</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
       <c r="D69" s="8">
-        <v>63123138</v>
+        <v>38928838</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>91</v>
@@ -3480,7 +3483,7 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>227</v>
+        <v>151</v>
       </c>
       <c r="J69">
         <v>2</v>
@@ -3488,16 +3491,16 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
       <c r="D70" s="8">
-        <v>23479239</v>
+        <v>77807493</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>74</v>
@@ -3512,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>229</v>
+        <v>153</v>
       </c>
       <c r="J70">
         <v>2</v>
@@ -3520,16 +3523,16 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" s="8">
-        <v>11352861</v>
+        <v>57115951</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>75</v>
@@ -3544,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="J71">
         <v>2</v>
@@ -3552,19 +3555,19 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>232</v>
+        <v>156</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
       <c r="D72" s="8">
-        <v>31361931</v>
+        <v>53592943</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F72">
         <v>6</v>
@@ -3576,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>233</v>
+        <v>157</v>
       </c>
       <c r="J72">
         <v>2</v>
@@ -3584,16 +3587,16 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>234</v>
+        <v>158</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
-      <c r="D73" s="8">
-        <v>93020326</v>
+      <c r="D73" s="8" t="s">
+        <v>323</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>76</v>
@@ -3608,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>235</v>
+        <v>159</v>
       </c>
       <c r="J73">
         <v>2</v>
@@ -3616,19 +3619,19 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>236</v>
+        <v>160</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" s="8">
-        <v>95376582</v>
+        <v>62141561</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="F74">
         <v>6</v>
@@ -3640,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>237</v>
+        <v>161</v>
       </c>
       <c r="J74">
         <v>2</v>
@@ -3648,16 +3651,16 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>238</v>
+        <v>162</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" s="8">
-        <v>81952034</v>
+        <v>90770017</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>77</v>
@@ -3672,7 +3675,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>239</v>
+        <v>163</v>
       </c>
       <c r="J75">
         <v>2</v>
@@ -3680,16 +3683,16 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>240</v>
+        <v>164</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
       <c r="D76" s="8">
-        <v>66530924</v>
+        <v>23357354</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>78</v>
@@ -3704,7 +3707,7 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>241</v>
+        <v>165</v>
       </c>
       <c r="J76">
         <v>2</v>
@@ -3712,19 +3715,19 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>242</v>
+        <v>166</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" s="8">
-        <v>41491837</v>
+        <v>22561141</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="F77">
         <v>6</v>
@@ -3736,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>243</v>
+        <v>167</v>
       </c>
       <c r="J77">
         <v>2</v>
@@ -3744,16 +3747,16 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>244</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
       <c r="D78" s="8">
-        <v>76730752</v>
+        <v>96671188</v>
       </c>
       <c r="E78" s="6" t="s">
         <v>79</v>
@@ -3768,7 +3771,7 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>245</v>
+        <v>169</v>
       </c>
       <c r="J78">
         <v>2</v>
@@ -3776,16 +3779,16 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>246</v>
+        <v>170</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C79">
         <v>1</v>
       </c>
       <c r="D79" s="8">
-        <v>96560776</v>
+        <v>78994810</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>80</v>
@@ -3800,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>247</v>
+        <v>171</v>
       </c>
       <c r="J79">
         <v>2</v>
@@ -3808,19 +3811,19 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>248</v>
+        <v>172</v>
       </c>
       <c r="B80" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C80">
         <v>1</v>
       </c>
       <c r="D80" s="8">
-        <v>18712761</v>
+        <v>81507611</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F80">
         <v>6</v>
@@ -3832,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="J80">
         <v>2</v>
@@ -3840,19 +3843,19 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>250</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C81">
         <v>3</v>
       </c>
       <c r="D81" s="8">
-        <v>74567593</v>
+        <v>53275431</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
+        <v>327</v>
       </c>
       <c r="F81">
         <v>10</v>
@@ -3864,24 +3867,24 @@
         <v>0</v>
       </c>
       <c r="I81" t="s">
-        <v>251</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>252</v>
+        <v>176</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C82">
         <v>3</v>
       </c>
       <c r="D82" s="8">
-        <v>84328556</v>
+        <v>18858100</v>
       </c>
       <c r="E82" t="s">
-        <v>110</v>
+        <v>328</v>
       </c>
       <c r="F82">
         <v>10</v>
@@ -3893,24 +3896,24 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>253</v>
+        <v>177</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>178</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C83">
         <v>3</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="E83" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="F83">
         <v>10</v>
@@ -3922,24 +3925,24 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>255</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>256</v>
+        <v>180</v>
       </c>
       <c r="B84" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C84">
         <v>3</v>
       </c>
       <c r="D84" s="8">
-        <v>69541953</v>
+        <v>92019584</v>
       </c>
       <c r="E84" t="s">
-        <v>112</v>
+        <v>330</v>
       </c>
       <c r="F84">
         <v>10</v>
@@ -3951,24 +3954,24 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>257</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>258</v>
+        <v>182</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C85">
         <v>3</v>
       </c>
       <c r="D85" s="8">
-        <v>62387771</v>
+        <v>72722985</v>
       </c>
       <c r="E85" t="s">
-        <v>113</v>
+        <v>331</v>
       </c>
       <c r="F85">
         <v>10</v>
@@ -3980,24 +3983,24 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>259</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>260</v>
+        <v>184</v>
       </c>
       <c r="B86" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C86">
         <v>3</v>
       </c>
       <c r="D86" s="8">
-        <v>75586895</v>
+        <v>34457088</v>
       </c>
       <c r="E86" t="s">
-        <v>114</v>
+        <v>332</v>
       </c>
       <c r="F86">
         <v>10</v>
@@ -4009,24 +4012,24 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>261</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>262</v>
+        <v>186</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C87">
         <v>3</v>
       </c>
       <c r="D87" s="8">
-        <v>82086884</v>
+        <v>82793794</v>
       </c>
       <c r="E87" t="s">
-        <v>115</v>
+        <v>333</v>
       </c>
       <c r="F87">
         <v>10</v>
@@ -4038,24 +4041,24 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>263</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>264</v>
+        <v>188</v>
       </c>
       <c r="B88" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C88">
         <v>3</v>
       </c>
-      <c r="D88" s="8">
-        <v>98132593</v>
+      <c r="D88" s="8" t="s">
+        <v>321</v>
       </c>
       <c r="E88" t="s">
-        <v>116</v>
+        <v>334</v>
       </c>
       <c r="F88">
         <v>10</v>
@@ -4067,24 +4070,24 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>265</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>266</v>
+        <v>190</v>
       </c>
       <c r="B89" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C89">
         <v>3</v>
       </c>
       <c r="D89" s="8">
-        <v>37519096</v>
+        <v>81447813</v>
       </c>
       <c r="E89" t="s">
-        <v>117</v>
+        <v>335</v>
       </c>
       <c r="F89">
         <v>10</v>
@@ -4096,24 +4099,24 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>267</v>
+        <v>191</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>268</v>
+        <v>192</v>
       </c>
       <c r="B90" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C90">
         <v>3</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>339</v>
+      <c r="D90" s="8">
+        <v>11644954</v>
       </c>
       <c r="E90" t="s">
-        <v>118</v>
+        <v>336</v>
       </c>
       <c r="F90">
         <v>10</v>
@@ -4125,24 +4128,24 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>269</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>194</v>
       </c>
       <c r="B91" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C91">
         <v>3</v>
       </c>
       <c r="D91" s="8">
-        <v>78748553</v>
+        <v>38739033</v>
       </c>
       <c r="E91" t="s">
-        <v>92</v>
+        <v>324</v>
       </c>
       <c r="F91">
         <v>10</v>
@@ -4154,24 +4157,24 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>271</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>196</v>
       </c>
       <c r="B92" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C92">
         <v>3</v>
       </c>
       <c r="D92" s="8">
-        <v>46355701</v>
+        <v>78742396</v>
       </c>
       <c r="E92" t="s">
-        <v>93</v>
+        <v>325</v>
       </c>
       <c r="F92">
         <v>10</v>
@@ -4183,24 +4186,24 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>273</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>274</v>
+        <v>198</v>
       </c>
       <c r="B93" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C93">
         <v>3</v>
       </c>
       <c r="D93" s="8">
-        <v>53341886</v>
+        <v>77553454</v>
       </c>
       <c r="E93" t="s">
-        <v>94</v>
+        <v>326</v>
       </c>
       <c r="F93">
         <v>10</v>
@@ -4212,24 +4215,24 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>275</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>276</v>
+        <v>200</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C94">
         <v>3</v>
       </c>
-      <c r="D94" s="8">
-        <v>44741835</v>
+      <c r="D94" s="8" t="s">
+        <v>320</v>
       </c>
       <c r="E94" t="s">
-        <v>95</v>
+        <v>337</v>
       </c>
       <c r="F94">
         <v>10</v>
@@ -4241,24 +4244,24 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>278</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C95">
         <v>3</v>
       </c>
-      <c r="D95" s="8" t="s">
-        <v>340</v>
+      <c r="D95" s="8">
+        <v>49789723</v>
       </c>
       <c r="E95" t="s">
-        <v>96</v>
+        <v>338</v>
       </c>
       <c r="F95">
         <v>10</v>
@@ -4270,24 +4273,24 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>279</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>280</v>
+        <v>204</v>
       </c>
       <c r="B96" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C96">
         <v>3</v>
       </c>
       <c r="D96" s="8">
-        <v>90991859</v>
+        <v>78867611</v>
       </c>
       <c r="E96" t="s">
-        <v>97</v>
+        <v>339</v>
       </c>
       <c r="F96">
         <v>10</v>
@@ -4299,24 +4302,24 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>281</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>282</v>
+        <v>206</v>
       </c>
       <c r="B97" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>3</v>
       </c>
-      <c r="D97" s="8">
-        <v>52739881</v>
+      <c r="D97" s="8" t="s">
+        <v>319</v>
       </c>
       <c r="E97" t="s">
-        <v>98</v>
+        <v>340</v>
       </c>
       <c r="F97">
         <v>10</v>
@@ -4328,24 +4331,24 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>283</v>
+        <v>207</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>284</v>
+        <v>208</v>
       </c>
       <c r="B98" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>3</v>
       </c>
       <c r="D98" s="8">
-        <v>90950994</v>
+        <v>61241224</v>
       </c>
       <c r="E98" t="s">
-        <v>99</v>
+        <v>341</v>
       </c>
       <c r="F98">
         <v>10</v>
@@ -4357,24 +4360,24 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>285</v>
+        <v>209</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>210</v>
       </c>
       <c r="B99" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C99">
         <v>3</v>
       </c>
       <c r="D99" s="8">
-        <v>45810217</v>
+        <v>85560945</v>
       </c>
       <c r="E99" t="s">
-        <v>100</v>
+        <v>342</v>
       </c>
       <c r="F99">
         <v>10</v>
@@ -4386,24 +4389,24 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>287</v>
+        <v>211</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>288</v>
+        <v>212</v>
       </c>
       <c r="B100" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C100">
         <v>3</v>
       </c>
       <c r="D100" s="8">
-        <v>74053845</v>
+        <v>41434856</v>
       </c>
       <c r="E100" t="s">
-        <v>101</v>
+        <v>343</v>
       </c>
       <c r="F100">
         <v>10</v>
@@ -4415,21 +4418,21 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>289</v>
+        <v>213</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>290</v>
+        <v>214</v>
       </c>
       <c r="B101" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C101">
         <v>3</v>
       </c>
       <c r="D101" s="8">
-        <v>22525202</v>
+        <v>38241344</v>
       </c>
       <c r="E101" t="s">
         <v>81</v>
@@ -4444,21 +4447,21 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>291</v>
+        <v>215</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>292</v>
+        <v>216</v>
       </c>
       <c r="B102" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C102">
         <v>3</v>
       </c>
       <c r="D102" s="8">
-        <v>98923842</v>
+        <v>86229793</v>
       </c>
       <c r="E102" t="s">
         <v>82</v>
@@ -4473,21 +4476,21 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>293</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>294</v>
+        <v>218</v>
       </c>
       <c r="B103" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C103">
         <v>3</v>
       </c>
       <c r="D103" s="8">
-        <v>75212742</v>
+        <v>10024586</v>
       </c>
       <c r="E103" t="s">
         <v>83</v>
@@ -4502,21 +4505,21 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>295</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>296</v>
+        <v>220</v>
       </c>
       <c r="B104" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C104">
         <v>3</v>
       </c>
       <c r="D104" s="8">
-        <v>37675836</v>
+        <v>14652780</v>
       </c>
       <c r="E104" t="s">
         <v>84</v>
@@ -4531,21 +4534,21 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>297</v>
+        <v>221</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>298</v>
+        <v>222</v>
       </c>
       <c r="B105" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C105">
         <v>3</v>
       </c>
       <c r="D105" s="8">
-        <v>46874412</v>
+        <v>35984703</v>
       </c>
       <c r="E105" t="s">
         <v>85</v>
@@ -4560,21 +4563,21 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>299</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>300</v>
+        <v>224</v>
       </c>
       <c r="B106" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C106">
         <v>3</v>
       </c>
       <c r="D106" s="8" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="E106" t="s">
         <v>86</v>
@@ -4589,21 +4592,21 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>301</v>
+        <v>225</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>302</v>
+        <v>226</v>
       </c>
       <c r="B107" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C107">
         <v>3</v>
       </c>
       <c r="D107" s="8">
-        <v>39823023</v>
+        <v>98367596</v>
       </c>
       <c r="E107" t="s">
         <v>87</v>
@@ -4618,21 +4621,21 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>303</v>
+        <v>227</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>304</v>
+        <v>228</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C108">
         <v>3</v>
       </c>
       <c r="D108" s="8">
-        <v>66301106</v>
+        <v>87295252</v>
       </c>
       <c r="E108" t="s">
         <v>88</v>
@@ -4647,21 +4650,21 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>305</v>
+        <v>229</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>306</v>
+        <v>230</v>
       </c>
       <c r="B109" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C109">
         <v>3</v>
       </c>
       <c r="D109" s="8">
-        <v>41179047</v>
+        <v>50963368</v>
       </c>
       <c r="E109" t="s">
         <v>89</v>
@@ -4676,21 +4679,21 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>307</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>308</v>
+        <v>232</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C110">
         <v>3</v>
       </c>
-      <c r="D110" s="8">
-        <v>38108918</v>
+      <c r="D110" s="8" t="s">
+        <v>317</v>
       </c>
       <c r="E110" t="s">
         <v>90</v>
@@ -4705,21 +4708,21 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>309</v>
+        <v>233</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>310</v>
+        <v>234</v>
       </c>
       <c r="B111" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C111">
         <v>3</v>
       </c>
       <c r="D111" s="8">
-        <v>61023692</v>
+        <v>92292186</v>
       </c>
       <c r="E111" t="s">
         <v>81</v>
@@ -4734,21 +4737,21 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>311</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>312</v>
+        <v>236</v>
       </c>
       <c r="B112" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
-      <c r="D112" s="8">
-        <v>87564015</v>
+      <c r="D112" s="8" t="s">
+        <v>316</v>
       </c>
       <c r="E112" t="s">
         <v>82</v>
@@ -4763,21 +4766,21 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>313</v>
+        <v>237</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>314</v>
+        <v>238</v>
       </c>
       <c r="B113" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C113">
         <v>3</v>
       </c>
       <c r="D113" s="8">
-        <v>78487124</v>
+        <v>25337936</v>
       </c>
       <c r="E113" t="s">
         <v>83</v>
@@ -4792,21 +4795,21 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>315</v>
+        <v>239</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>316</v>
+        <v>240</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C114">
         <v>3</v>
       </c>
       <c r="D114" s="8">
-        <v>42813248</v>
+        <v>76335627</v>
       </c>
       <c r="E114" t="s">
         <v>84</v>
@@ -4821,21 +4824,21 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>317</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>318</v>
+        <v>242</v>
       </c>
       <c r="B115" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C115">
         <v>3</v>
       </c>
-      <c r="D115" s="8" t="s">
-        <v>342</v>
+      <c r="D115" s="8">
+        <v>32826558</v>
       </c>
       <c r="E115" t="s">
         <v>85</v>
@@ -4850,21 +4853,21 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>319</v>
+        <v>243</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>320</v>
+        <v>244</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C116">
         <v>3</v>
       </c>
-      <c r="D116" s="8">
-        <v>81199577</v>
+      <c r="D116" s="8" t="s">
+        <v>315</v>
       </c>
       <c r="E116" t="s">
         <v>86</v>
@@ -4879,21 +4882,21 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>321</v>
+        <v>245</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>322</v>
+        <v>246</v>
       </c>
       <c r="B117" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C117">
         <v>3</v>
       </c>
       <c r="D117" s="8">
-        <v>65840612</v>
+        <v>66443310</v>
       </c>
       <c r="E117" t="s">
         <v>87</v>
@@ -4908,21 +4911,21 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>323</v>
+        <v>247</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>324</v>
+        <v>248</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C118">
         <v>3</v>
       </c>
       <c r="D118" s="8">
-        <v>19901803</v>
+        <v>54424269</v>
       </c>
       <c r="E118" t="s">
         <v>88</v>
@@ -4937,21 +4940,21 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>325</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>326</v>
+        <v>250</v>
       </c>
       <c r="B119" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C119">
         <v>3</v>
       </c>
       <c r="D119" s="8">
-        <v>65082633</v>
+        <v>51265695</v>
       </c>
       <c r="E119" t="s">
         <v>89</v>
@@ -4966,21 +4969,21 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>327</v>
+        <v>251</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>328</v>
+        <v>252</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C120">
         <v>3</v>
       </c>
       <c r="D120" s="8">
-        <v>70937939</v>
+        <v>65120941</v>
       </c>
       <c r="E120" t="s">
         <v>90</v>
@@ -4995,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>329</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>